<commit_message>
Mern ai project for internship
</commit_message>
<xml_diff>
--- a/backend/outputs/Horizon Capital_Extracted.xlsx
+++ b/backend/outputs/Horizon Capital_Extracted.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Page 1, opening letter (signed by Evelyn Reed, General Partner)</t>
+          <t>Page 1, opening letter (Signed by Evelyn Reed, Horizon Capital Partners I Limited, the General Partner to Horizon Growth Fund I L.P.)</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,7 +482,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Page 1 (letterhead) and Page 2 (fund association with Zenith Innovations)</t>
+          <t>Page 1, opening letter (Header: 'Horizon Growth Fund I L.P. - 1st Quarter 2024 Report')</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -502,7 +502,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Page 2 (Zenith Innovations: 'Currency: US$') and Page 6 (financial statements in USD)</t>
+          <t>Page 2 (Zenith Innovations: 'Currency: US$ (in millions)') and Page 6 (Financial statements in USD)</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -522,7 +522,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Derived: No explicit mention of total commitments in document.</t>
+          <t>Pages 1-8 (No mention of total commitments or fund size)</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Derived: No breakdown of drawdowns provided. Only invested capital per company is listed (e.g., 75M for Zenith).</t>
+          <t>Pages 1-8 (No breakdown of drawdowns/capital calls)</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Derived: Insufficient data to calculate (requires Total Commitments - Total Drawdowns).</t>
+          <t>Pages 1-8 (No data on unused commitments)</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -577,16 +577,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1.25M</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Realised Value' = 0 for all investments) and Page 2/4 ('Capital Returned: 0').</t>
+          <t>Page 6 (Income statement: 'Dividend Income 1,250,000.00')</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +602,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Page 8 (Realised Value = 0 / Invested Capital = 75M for Zenith; no other investments listed). Calculated as: 0 / 75M = 0.00x.</t>
+          <t>Page 8 (Zenith Innovations: 'Realised Value: 0' and 'Total Fund I Investments - Gross' shows no distributions)</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -622,11 +622,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Multiple of Investment' = 1.53x for Zenith). Assumed to represent RVPI (Unrealised Value / Invested Capital).</t>
+          <t>Page 8 (Zenith Innovations: 'Total Value: 115,000' vs 'Invested Capital: 75,000' → 115/75 = 1.53x)</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -642,7 +642,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Multiple of Investment' = 1.53x). Confirmed as TVPI = (Realised + Unrealised) / Invested = (0 + 115M) / 75M = 1.53x.</t>
+          <t>Page 8 (Zenith Innovations: 'Multiple of Investment: 1.53x' and no other investments listed)</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -662,7 +662,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Page 8 (only Gross IRR = 25.0% provided; Net IRR not disclosed).</t>
+          <t>Pages 1-8 (Only Gross IRR of 25.0% provided; no net IRR disclosed)</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -682,7 +682,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Gross IRR' = 25.0%).</t>
+          <t>Page 8 (Zenith Innovations: 'Gross IRR: 25.0%')</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -695,18 +695,16 @@
           <t>Number of Investments</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B14" t="n">
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Pages 2–5 (Zenith Innovations, EcoHarvest Solutions). Page 8 confirms only Zenith is active in Fund I (EcoHarvest may be in a different vehicle or not yet fully reported).</t>
+          <t>Pages 2-5 (Zenith Innovations Ltd. and EcoHarvest Solutions Inc. listed; Page 8 confirms only Zenith in 'Total Fund I Investments' but EcoHarvest is detailed in Pages 4-5)</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -715,14 +713,12 @@
           <t>Active Portfolio Companies</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="B15" t="n">
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table lists only Zenith Innovations as 'Active'). EcoHarvest's status not explicitly stated in Fund I context.</t>
+          <t>Pages 2-5 (Both Zenith Innovations and EcoHarvest Solutions marked as 'Active' or with 'Latest Quarter' updates)</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -742,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Page 2 (company header)</t>
+          <t>Page 2 (Header: 'Zenith Innovations Ltd.')</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -762,7 +758,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Page 2 ('Date of Inv: December 2021')</t>
+          <t>Page 2 ('Date of Inv: December 2021') and Page 8 ('Investment Date: Dec 2021')</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -802,7 +798,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Page 2 ('Invested Capital: 75') and Page 8 (Investment Performance table: 'Invested Capital' = 75,000 in thousands)</t>
+          <t>Page 2 ('Invested Capital: 75') and Page 8 ('Invested Capital: 75,000 [in thousands]')</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -842,7 +838,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Total Value' = 115,000 in thousands).</t>
+          <t>Page 8 ('Unrealised Value: 115,000 [in thousands]')</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -862,7 +858,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Page 8 (Investment Performance table: 'Status' = Active)</t>
+          <t>Page 8 ('Exit Status: Active')</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -882,7 +878,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Page 4 (company header)</t>
+          <t>Page 4 (Header: 'EcoHarvest Solutions Inc.')</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -942,11 +938,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Page 4 ('Invested Capital: 60'). Note: Not listed in Fund I performance table (Page 8), suggesting possible exclusion or different fund vehicle.</t>
+          <t>Page 4 ('Invested Capital: 60')</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27">
@@ -982,7 +978,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Derived: Not included in Fund I performance table (Page 8). No unrealised/realised values provided for EcoHarvest in this report.</t>
+          <t>Pages 1-8 (No unrealised/realised value provided for EcoHarvest; Page 8 only lists Zenith)</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -997,16 +993,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Derived: Status not explicitly stated for EcoHarvest in Fund I context (Page 8 only lists Zenith).</t>
+          <t>Page 4 ('Latest Quarter: Q3 2024' implies ongoing activity; no exit mentioned)</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>